<commit_message>
Update test cases and Add collection test cases
</commit_message>
<xml_diff>
--- a/TestData/DigitalCodes data.xlsx
+++ b/TestData/DigitalCodes data.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20400" windowHeight="7815"/>
+    <workbookView windowWidth="20400" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Titles" sheetId="1" r:id="rId1"/>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
     <sheet name="Invalid Users" sheetId="3" r:id="rId3"/>
+    <sheet name="Collection" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Section</t>
   </si>
@@ -148,6 +149,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>CHAPTER 1 GENERAL</t>
+  </si>
+  <si>
+    <t>2023 Energy Collection</t>
+  </si>
+  <si>
+    <t>2021 CFR Part 3285 Model Manufactured Home Installation Standards</t>
+  </si>
+  <si>
+    <t>Subpart C— Site Preparation</t>
   </si>
 </sst>
 </file>
@@ -155,12 +171,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +193,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -191,9 +238,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,31 +268,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,6 +282,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -268,8 +336,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -278,43 +353,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,13 +377,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -350,55 +397,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,127 +577,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,17 +602,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,11 +645,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,17 +669,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,15 +708,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -679,147 +726,165 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1146,8 +1211,8 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="19" customHeight="1" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1173,100 +1238,100 @@
       </c>
     </row>
     <row r="2" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1308,16 +1373,16 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1351,34 +1416,34 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1394,4 +1459,69 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="11.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="26.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="90.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="29.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new test cases for collection and basic title
</commit_message>
<xml_diff>
--- a/TestData/DigitalCodes data.xlsx
+++ b/TestData/DigitalCodes data.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20400" windowHeight="7815" activeTab="3"/>
+    <workbookView windowWidth="20400" windowHeight="7815" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Titles" sheetId="1" r:id="rId1"/>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
     <sheet name="Invalid Users" sheetId="3" r:id="rId3"/>
     <sheet name="Collection" sheetId="4" r:id="rId4"/>
+    <sheet name="Basic" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Section</t>
   </si>
@@ -164,6 +165,12 @@
   </si>
   <si>
     <t>Subpart C— Site Preparation</t>
+  </si>
+  <si>
+    <t>Wiley</t>
+  </si>
+  <si>
+    <t>2021 Building Codes Illustrated, 7th Edition</t>
   </si>
 </sst>
 </file>
@@ -171,10 +178,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -238,42 +245,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -282,17 +253,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,35 +346,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -343,40 +367,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -397,85 +404,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,97 +584,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -606,6 +613,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -621,15 +652,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -641,6 +663,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -671,15 +702,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -688,35 +710,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -726,134 +733,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -863,6 +870,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -886,9 +899,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1211,8 +1221,8 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="19" customHeight="1" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1238,100 +1248,100 @@
       </c>
     </row>
     <row r="2" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1373,16 +1383,16 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1416,34 +1426,34 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1466,8 +1476,8 @@
   <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -1499,10 +1509,10 @@
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1510,14 +1520,58 @@
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="12.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create ASTM test cases
</commit_message>
<xml_diff>
--- a/TestData/DigitalCodes data.xlsx
+++ b/TestData/DigitalCodes data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20400" windowHeight="7815"/>
+    <workbookView windowWidth="20400" windowHeight="7815" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Titles" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Invalid Users" sheetId="3" r:id="rId3"/>
     <sheet name="Collection" sheetId="4" r:id="rId4"/>
     <sheet name="Basic" sheetId="5" r:id="rId5"/>
+    <sheet name="ASTM" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>Section</t>
   </si>
@@ -171,6 +172,21 @@
   </si>
   <si>
     <t>2021 Building Codes Illustrated, 7th Edition</t>
+  </si>
+  <si>
+    <t>Categoray</t>
+  </si>
+  <si>
+    <t>ASTM Standards</t>
+  </si>
+  <si>
+    <t>Iron and Steel Materials</t>
+  </si>
+  <si>
+    <t>ASTM A1003/A1003M-15</t>
+  </si>
+  <si>
+    <t>A1003/A1003M-15</t>
   </si>
 </sst>
 </file>
@@ -178,10 +194,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -259,34 +275,88 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -298,92 +368,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,187 +420,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,15 +629,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -642,30 +649,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -700,6 +683,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -715,15 +731,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -733,139 +749,142 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1215,8 +1234,8 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="19" customHeight="1" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1420,34 +1439,34 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1471,7 +1490,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -1503,10 +1522,10 @@
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1514,13 +1533,13 @@
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1536,7 +1555,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1561,11 +1580,69 @@
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="24.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="24.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="35.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="18.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>